<commit_message>
update qft sqrt2 results
</commit_message>
<xml_diff>
--- a/results/yq_test/GHZ_cz/Rb2Re4/GHZ_cz_total.xlsx
+++ b/results/yq_test/GHZ_cz/Rb2Re4/GHZ_cz_total.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentutsedu-my.sharepoint.com/personal/yunqi_huang_student_uts_edu_au/Documents/Untitled Folder/NAQCT/results/yq_test/GHZ_cz/Rb2Re4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_63C545BCDD2AD466A983C8F0505ED87656CDD4AD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9016FF7E-DAE2-F540-B278-8BC8EC0DA67B}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_63C545BCDD2AD466A983C8F0505ED87656CDD4AD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9F1D2D8-467E-3F43-90FD-00D1ECE3DA18}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet!$B$2:$B$47</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet!$E$2:$E$47</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet!$B$2:$B$47</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet!$E$2:$E$47</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1948,16 +1942,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>336550</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2272,8 +2266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E2" activeCellId="1" sqref="B2:B47 E2:E47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>

</xml_diff>